<commit_message>
dodat json podaci i promenjena struktura projekta
</commit_message>
<xml_diff>
--- a/Bug Tracing.xlsx
+++ b/Bug Tracing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="62">
   <si>
     <t>ID Test scenaria</t>
   </si>
@@ -196,6 +196,21 @@
   <si>
     <t>Neuspesan login</t>
   </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>Provera funkcionalnosti Log In Forme</t>
+  </si>
+  <si>
+    <t>LogInForma</t>
+  </si>
+  <si>
+    <t>Provera funckionalosti LogIn forme</t>
+  </si>
+  <si>
+    <t>Aleksandra Adamovic</t>
+  </si>
 </sst>
 </file>
 
@@ -360,6 +375,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -381,10 +400,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,33 +637,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="18"/>
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="18"/>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
@@ -656,37 +671,37 @@
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="13" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="13" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="13" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="16"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="20"/>
       <c r="T5" s="3"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
@@ -1879,17 +1894,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -1901,149 +1916,149 @@
       <c r="C2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="str">
+      <c r="A3" s="27" t="str">
         <f>TestScenarioReg!C1</f>
         <v>RegistracionaForma</v>
       </c>
-      <c r="B3" s="24" t="str">
+      <c r="B3" s="28" t="str">
         <f>TestScenarioReg!F1</f>
         <v>Provera funckionalosti registracione forme</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="D4" s="18" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="D4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="16"/>
-      <c r="D5" s="18" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="D5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="16"/>
-      <c r="D6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="D6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
-      <c r="D7" s="18" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="20"/>
+      <c r="D7" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="18" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="D8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="18" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="20"/>
+      <c r="D9" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="D10" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16"/>
-      <c r="D11" s="18" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="D11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="20"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3028,18 +3043,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="D2:F2"/>
@@ -3050,6 +3053,18 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3063,7 +3078,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3079,33 +3094,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="18"/>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3113,37 +3131,37 @@
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="13" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="13" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="13" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="16"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="20"/>
       <c r="T5" s="3"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
@@ -4323,7 +4341,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4338,17 +4356,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -4360,174 +4378,193 @@
       <c r="C2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="28" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="str">
-        <f>TestScenarioReg!C1</f>
-        <v>RegistracionaForma</v>
-      </c>
-      <c r="B3" s="24" t="str">
-        <f>TestScenarioReg!F1</f>
-        <v>Provera funckionalosti registracione forme</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="A3" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="H3" s="27" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="H3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="D4" s="18" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="D4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="H4" s="27" t="s">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="H4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="16"/>
-      <c r="D5" s="18" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="D5" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="H5" s="14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="16"/>
-      <c r="D6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="D6" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="20"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="18" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="D8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="18" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="20"/>
+      <c r="D9" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="D10" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16"/>
-      <c r="D11" s="18" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="D11" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="18" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="D12" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="20"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="20"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5512,6 +5549,12 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="D2:F2"/>
@@ -5519,11 +5562,6 @@
     <mergeCell ref="B3:B15"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
@@ -5533,7 +5571,6 @@
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5564,33 +5601,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="18"/>
+      <c r="D2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="18"/>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
@@ -5598,37 +5635,37 @@
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="13" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="13" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="13" t="s">
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="16"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="20"/>
       <c r="T5" s="3"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
@@ -6821,17 +6858,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -6843,149 +6880,149 @@
       <c r="C2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="str">
+      <c r="A3" s="27" t="str">
         <f>TestScenarioReg!C1</f>
         <v>RegistracionaForma</v>
       </c>
-      <c r="B3" s="24" t="str">
+      <c r="B3" s="28" t="str">
         <f>TestScenarioReg!F1</f>
         <v>Provera funckionalosti registracione forme</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16"/>
-      <c r="D4" s="18" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="D4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="16"/>
-      <c r="D5" s="18" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="20"/>
+      <c r="D5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="16"/>
-      <c r="D6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="20"/>
+      <c r="D6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
-      <c r="D7" s="18" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="20"/>
+      <c r="D7" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16"/>
-      <c r="D8" s="18" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+      <c r="D8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16"/>
-      <c r="D9" s="18" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="20"/>
+      <c r="D9" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16"/>
-      <c r="D10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="20"/>
+      <c r="D10" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16"/>
-      <c r="D11" s="18" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="20"/>
+      <c r="D11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="20"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="4:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7970,18 +8007,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="D2:F2"/>
@@ -7992,6 +8017,18 @@
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>